<commit_message>
2023-11-02 22:40:07 Update Excel file
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\10-31\data\20231031_superdelivery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\10-31\data\20231102_superdelivery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF4F83F-63D3-4A25-8131-043E6271AE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4C7FB3-AEC0-462A-82F9-576136C33B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="615" windowWidth="21600" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="420" windowWidth="25125" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>規劃時間</t>
   </si>
@@ -40,29 +40,39 @@
     <t>127520840434805,103482326003878,17841461742288388,17841456036806884</t>
   </si>
   <si>
-    <t>C:/Users/user/Desktop/10-31/data/20231031_superdelivery\【日本直送】 OMNES  メンズ　ふわ軽静電気防止　マイクロフリースパンツ　2023秋冬新作  男士蓬鬆輕薄防靜電微絨長褲 2023 秋冬新款  八色入</t>
-  </si>
-  <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_29567590827170513294.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_60376645994529596215.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_77666221561243252646.jpg</t>
-  </si>
-  <si>
-    <t>C:/Users/user/Desktop/10-31/data/20231031_superdelivery\【日本直送】 SAFARI ROOKIE  イージーパンツ メンズ ストレッチ 裏起毛 スーパーストレッチパンツ チノパン カジュアル ゴルフ ビジネス  Easy Pants 男士彈性羊毛襯裡超彈性褲子奇諾褲休閒高爾夫商務  八色入</t>
-  </si>
-  <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_94201058986672985450.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_54378725694341996175.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_66840199919010171874.jpg</t>
-  </si>
-  <si>
-    <t>C:/Users/user/Desktop/10-31/data/20231031_superdelivery\【日本直送】 improves　インプローブス  【SIDEWAYSTANCE】デニムケミカルワイドカーゴパンツ  [SIDEWAYSTANCE] 牛仔化纖寬幅工裝褲  二色入</t>
-  </si>
-  <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_75483551238368134853.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_42444143257935562217.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_21411498476000819587.jpg</t>
+    <t>C:/Users/user/Desktop/10-31/data/20231102_superdelivery\【日本直送】 QUASH(クワッシュ)(QUBJM)  飛びヒゲ刺繍スウェット（長袖スウェット）【2023年秋冬物新作商品】  飛須刺繡衛衣（長袖衛衣）【2023秋冬新品】  一色入</t>
+  </si>
+  <si>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_08082744085599597628.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_54978859891964370052.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_66281112341504638319.jpg</t>
+  </si>
+  <si>
+    <t>C:/Users/user/Desktop/10-31/data/20231102_superdelivery\【日本直送】 BARCEDOS  【2023秋冬】＜選べる9タイプ＞ロゴプリント 長袖Tシャツ  【2023秋冬】9款可選Logo印花長袖T卹  九色入</t>
+  </si>
+  <si>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_56914594841313592411.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_58518174693109314285.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_41273738738784776379.jpg</t>
+  </si>
+  <si>
+    <t>C:/Users/user/Desktop/10-31/data/20231102_superdelivery\【日本直送】 OMNES  メンズ　ダブルガーゼ　ポケット付き長袖Tシャツ　2023秋冬新作  男款雙層紗布長袖 T 卹（附口袋）2023 秋冬新款  十色入</t>
+  </si>
+  <si>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_53345774561473980927.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_99552404725753039171.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_42660133096556431775.jpg</t>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +86,13 @@
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,9 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -405,15 +423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="100.42578125" customWidth="1"/>
-    <col min="3" max="3" width="259.42578125" customWidth="1"/>
+    <col min="3" max="3" width="220.42578125" customWidth="1"/>
     <col min="4" max="4" width="367.42578125" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
   </cols>
@@ -435,9 +453,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45230.857638888891</v>
+        <v>45232.992361111108</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -448,10 +466,13 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>45230.85833333333</v>
+        <v>45232.992361111108</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -462,10 +483,13 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45230.859027777777</v>
+        <v>45232.992361111108</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -475,6 +499,9 @@
       </c>
       <c r="D4" t="s">
         <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023-11-19 05:58:55 Update Excel file
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\10-31\data\20231105_superdelivery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAEA0B2-7339-4C1B-A982-834ACE45667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2257E3CD-D409-4FB5-95C8-CB422E37D7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16297" yWindow="-5903" windowWidth="16395" windowHeight="28396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -8666,8 +8666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="41" zoomScaleNormal="41" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8970,7 +8970,7 @@
     </row>
     <row r="18" spans="1:5" ht="274.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45248.895833333336</v>
+        <v>45249.895833333336</v>
       </c>
       <c r="B18" t="s">
         <v>139</v>
@@ -9395,7 +9395,7 @@
     </row>
     <row r="43" spans="1:5" ht="273.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>45248.8125</v>
+        <v>45249.8125</v>
       </c>
       <c r="B43" t="s">
         <v>139</v>

</xml_diff>